<commit_message>
realizado importacao de excel para BD
</commit_message>
<xml_diff>
--- a/Planilhas/PlanilhaGELOMarcos.xlsx
+++ b/Planilhas/PlanilhaGELOMarcos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\Projeto GELO\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\Projeto-GELO\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718B3E71-AD62-436F-B6AB-D3538557E261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A2A94A-C8C7-4105-8E3B-611FD211C865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AD4D4DD5-5EC5-4070-A47B-2779E8EF634E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AD4D4DD5-5EC5-4070-A47B-2779E8EF634E}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{458EC5A9-C7A5-4A41-B3AC-F61CF4164E16}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7911B616-88A3-4A8F-BCE4-2DD0369637FD}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>